<commit_message>
before merging suite2p branch
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>mouse</t>
   </si>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,6 +581,30 @@
         <v>150</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1329</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1329</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1329</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
using improved ops to run suite2p segmentation
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>mouse</t>
   </si>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,6 +605,24 @@
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1337</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
trying compare registration shift btw ours & suite2p
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>mouse</t>
   </si>
@@ -36,12 +36,15 @@
   <si>
     <t>depth</t>
   </si>
+  <si>
+    <t>num</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +63,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,9 +92,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +422,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1322</v>
       </c>
@@ -427,7 +440,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1322</v>
       </c>
@@ -441,7 +454,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1322</v>
       </c>
@@ -455,7 +468,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1323</v>
       </c>
@@ -469,7 +482,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1323</v>
       </c>
@@ -483,7 +496,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1323</v>
       </c>
@@ -497,7 +510,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1324</v>
       </c>
@@ -511,7 +524,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1324</v>
       </c>
@@ -525,7 +538,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1328</v>
       </c>
@@ -539,7 +552,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1328</v>
       </c>
@@ -553,7 +566,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1328</v>
       </c>
@@ -563,11 +576,11 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1328</v>
       </c>
@@ -581,46 +594,182 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1329</v>
       </c>
+      <c r="B14">
+        <v>201209</v>
+      </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1329</v>
       </c>
+      <c r="B15">
+        <v>201217</v>
+      </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <v>200</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1329</v>
       </c>
+      <c r="B16">
+        <v>201217</v>
+      </c>
       <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>150</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1329</v>
+      </c>
+      <c r="B17">
+        <v>210113</v>
+      </c>
+      <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>200</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
+        <v>1329</v>
+      </c>
+      <c r="B18">
+        <v>210113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>150</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>1337</v>
       </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>210120</v>
+      </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>200</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1337</v>
+      </c>
+      <c r="B20">
+        <v>210120</v>
+      </c>
       <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>150</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1337</v>
+      </c>
+      <c r="B21">
+        <v>210127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>200</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1337</v>
+      </c>
+      <c r="B22">
+        <v>210127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>150</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1337</v>
+      </c>
+      <c r="B23">
+        <v>210203</v>
+      </c>
+      <c r="C23" t="s">
         <v>5</v>
+      </c>
+      <c r="D23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1337</v>
+      </c>
+      <c r="B24">
+        <v>210203</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor to allow mat -> py after init analysis
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="670" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
   <si>
     <t>mouse</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>num</t>
+  </si>
+  <si>
+    <t>seg</t>
+  </si>
+  <si>
+    <t>segmented</t>
+  </si>
+  <si>
+    <t>suite2p</t>
+  </si>
+  <si>
+    <t>seg_test</t>
   </si>
 </sst>
 </file>
@@ -401,15 +413,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="12.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +440,14 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1322</v>
       </c>
@@ -439,8 +460,14 @@
       <c r="D2">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1322</v>
       </c>
@@ -453,8 +480,11 @@
       <c r="D3">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1322</v>
       </c>
@@ -467,8 +497,11 @@
       <c r="D4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1323</v>
       </c>
@@ -481,8 +514,11 @@
       <c r="D5">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1323</v>
       </c>
@@ -495,8 +531,11 @@
       <c r="D6">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1323</v>
       </c>
@@ -509,8 +548,11 @@
       <c r="D7">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1324</v>
       </c>
@@ -523,8 +565,14 @@
       <c r="D8">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1324</v>
       </c>
@@ -537,8 +585,11 @@
       <c r="D9">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1328</v>
       </c>
@@ -552,7 +603,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1328</v>
       </c>
@@ -566,7 +617,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1328</v>
       </c>
@@ -580,7 +631,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1328</v>
       </c>
@@ -594,7 +645,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1329</v>
       </c>
@@ -607,8 +658,11 @@
       <c r="D14">
         <v>200</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1329</v>
       </c>
@@ -625,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1329</v>
       </c>

</xml_diff>

<commit_message>
added combined metrics (OSI+R2 thresholding) to define well fit. plotted tuning bias by area
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="24">
   <si>
     <t>mouse</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>007</t>
+  </si>
+  <si>
+    <t>forsaken?</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,6 +794,9 @@
       <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
@@ -810,6 +816,9 @@
       </c>
       <c r="E15" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
cut image to pieces of specific pixel size
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="27">
   <si>
     <t>mouse</t>
   </si>
@@ -49,9 +49,6 @@
     <t>suite2p</t>
   </si>
   <si>
-    <t>seg_test</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>007</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>gcamp</t>
   </si>
   <si>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>todo</t>
+  </si>
+  <si>
+    <t>suite2p_test</t>
+  </si>
+  <si>
+    <t>bad seg</t>
   </si>
 </sst>
 </file>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +519,9 @@
     <col min="5" max="5" width="8.88671875" style="4"/>
     <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="12.5546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -542,13 +544,13 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -568,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
@@ -594,10 +596,10 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -617,10 +619,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -640,10 +642,10 @@
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -663,10 +665,10 @@
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -686,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -709,10 +711,10 @@
         <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>10</v>
@@ -735,10 +737,10 @@
         <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -756,13 +758,13 @@
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -779,16 +781,16 @@
         <v>200</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -805,16 +807,16 @@
         <v>200</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -831,16 +833,16 @@
         <v>200</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -857,16 +859,16 @@
         <v>200</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -883,16 +885,16 @@
         <v>150</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -909,22 +911,22 @@
         <v>200</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1329</v>
       </c>
@@ -938,16 +940,16 @@
         <v>200</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1329</v>
       </c>
@@ -961,16 +963,16 @@
         <v>150</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1329</v>
       </c>
@@ -984,16 +986,16 @@
         <v>200</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1329</v>
       </c>
@@ -1007,16 +1009,16 @@
         <v>150</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1337</v>
       </c>
@@ -1030,16 +1032,19 @@
         <v>200</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1337</v>
       </c>
@@ -1053,16 +1058,16 @@
         <v>150</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1337</v>
       </c>
@@ -1076,16 +1081,16 @@
         <v>200</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1337</v>
       </c>
@@ -1099,16 +1104,16 @@
         <v>150</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1337</v>
       </c>
@@ -1122,16 +1127,16 @@
         <v>200</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1337</v>
       </c>
@@ -1145,16 +1150,16 @@
         <v>150</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1338</v>
       </c>
@@ -1168,16 +1173,16 @@
         <v>200</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1338</v>
       </c>
@@ -1191,16 +1196,16 @@
         <v>150</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1338</v>
       </c>
@@ -1214,16 +1219,16 @@
         <v>200</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1338</v>
       </c>
@@ -1237,16 +1242,16 @@
         <v>200</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>1338</v>
       </c>
@@ -1260,19 +1265,19 @@
         <v>200</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>1338</v>
       </c>
@@ -1286,19 +1291,19 @@
         <v>200</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1338</v>
       </c>
@@ -1312,16 +1317,19 @@
         <v>200</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33303</v>
       </c>
@@ -1335,17 +1343,17 @@
         <v>150</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33303</v>
       </c>
@@ -1359,16 +1367,16 @@
         <v>150</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>33303</v>
       </c>
@@ -1382,16 +1390,16 @@
         <v>150</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>33303</v>
       </c>
@@ -1405,16 +1413,16 @@
         <v>200</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>33303</v>
       </c>
@@ -1428,16 +1436,16 @@
         <v>200</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>33303</v>
       </c>
@@ -1451,19 +1459,19 @@
         <v>150</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>33303</v>
       </c>
@@ -1477,16 +1485,16 @@
         <v>200</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>33303</v>
       </c>
@@ -1500,19 +1508,22 @@
         <v>150</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>33303</v>
       </c>
@@ -1526,16 +1537,16 @@
         <v>200</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>33303</v>
       </c>
@@ -1549,19 +1560,19 @@
         <v>150</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>33303</v>
       </c>
@@ -1575,19 +1586,19 @@
         <v>200</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>33303</v>
       </c>
@@ -1601,19 +1612,19 @@
         <v>150</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>33303</v>
       </c>
@@ -1627,19 +1638,19 @@
         <v>150</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>33303</v>
       </c>
@@ -1653,13 +1664,13 @@
         <v>150</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reproduced mwork gaussian mask
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="28">
   <si>
     <t>mouse</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>bad seg</t>
+  </si>
+  <si>
+    <t>AWS</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +197,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +530,7 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,8 +558,11 @@
       <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1322</v>
       </c>
@@ -579,7 +588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1322</v>
       </c>
@@ -601,8 +610,11 @@
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1322</v>
       </c>
@@ -624,8 +636,11 @@
       <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1323</v>
       </c>
@@ -647,8 +662,11 @@
       <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1323</v>
       </c>
@@ -670,8 +688,11 @@
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1323</v>
       </c>
@@ -693,8 +714,11 @@
       <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1324</v>
       </c>
@@ -720,7 +744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1324</v>
       </c>
@@ -742,8 +766,11 @@
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1324</v>
       </c>
@@ -766,8 +793,11 @@
       <c r="H10" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1328</v>
       </c>
@@ -792,8 +822,11 @@
       <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1328</v>
       </c>
@@ -818,8 +851,11 @@
       <c r="H12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1328</v>
       </c>
@@ -844,8 +880,11 @@
       <c r="H13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1328</v>
       </c>
@@ -870,8 +909,11 @@
       <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1328</v>
       </c>
@@ -896,8 +938,11 @@
       <c r="H15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1329</v>
       </c>
@@ -1251,175 +1296,105 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>1338</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="9">
+        <v>210805</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1">
+        <v>150</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>1338</v>
+      </c>
+      <c r="B35" s="5">
         <v>210602</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="5">
-        <v>200</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="C35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5">
+        <v>200</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="H35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
         <v>1338</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B36" s="5">
         <v>210609</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="5">
-        <v>200</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="5" t="s">
+      <c r="C36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5">
+        <v>200</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+      <c r="H36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>1338</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B37" s="2">
         <v>210616</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="2">
-        <v>200</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>200</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B34" s="1">
-        <v>210401</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1">
-        <v>150</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B35" s="1">
-        <v>210405</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="1">
-        <v>150</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B36" s="1">
-        <v>210415</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="1">
-        <v>150</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B37" s="1">
-        <v>210415</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1">
-        <v>200</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1427,17 +1402,18 @@
         <v>33303</v>
       </c>
       <c r="B38" s="1">
-        <v>210419</v>
+        <v>210401</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F38" s="5"/>
       <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
@@ -1449,20 +1425,17 @@
       <c r="A39" s="1">
         <v>33303</v>
       </c>
-      <c r="B39" s="8">
-        <v>210419</v>
+      <c r="B39" s="1">
+        <v>210405</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="1">
         <v>150</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>18</v>
@@ -1476,13 +1449,13 @@
         <v>33303</v>
       </c>
       <c r="B40" s="1">
-        <v>210422</v>
+        <v>210415</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>11</v>
@@ -1498,37 +1471,31 @@
       <c r="A41" s="1">
         <v>33303</v>
       </c>
-      <c r="B41" s="8">
-        <v>210422</v>
+      <c r="B41" s="1">
+        <v>210415</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="8">
-        <v>150</v>
+      <c r="D41" s="1">
+        <v>200</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>33303</v>
       </c>
-      <c r="B42" s="2">
-        <v>210430</v>
+      <c r="B42" s="1">
+        <v>210419</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
@@ -1550,17 +1517,17 @@
       <c r="A43" s="1">
         <v>33303</v>
       </c>
-      <c r="B43" s="3">
-        <v>210430</v>
+      <c r="B43" s="8">
+        <v>210419</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="8">
         <v>150</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>24</v>
@@ -1576,20 +1543,17 @@
       <c r="A44" s="1">
         <v>33303</v>
       </c>
-      <c r="B44" s="3">
-        <v>210506</v>
+      <c r="B44" s="1">
+        <v>210422</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="1">
         <v>200</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>18</v>
@@ -1603,7 +1567,7 @@
         <v>33303</v>
       </c>
       <c r="B45" s="8">
-        <v>210603</v>
+        <v>210422</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
@@ -1612,7 +1576,7 @@
         <v>150</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>24</v>
@@ -1622,26 +1586,26 @@
       </c>
       <c r="H45" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>33303</v>
       </c>
-      <c r="B46" s="8">
-        <v>210610</v>
+      <c r="B46" s="2">
+        <v>210430</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="8">
-        <v>150</v>
+      <c r="D46" s="1">
+        <v>200</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>18</v>
@@ -1654,22 +1618,126 @@
       <c r="A47" s="1">
         <v>33303</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="3">
+        <v>210430</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="3">
+        <v>150</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B48" s="3">
+        <v>210506</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3">
+        <v>200</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B49" s="8">
+        <v>210603</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="8">
+        <v>150</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B50" s="8">
+        <v>210610</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="8">
+        <v>150</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B51" s="1">
         <v>210617</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="1">
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
         <v>150</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="1" t="s">
+      <c r="E51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remake fig for poster: adp mag
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10040009-FA77-46C2-A3D3-E2BF63286BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1236" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="1956" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="30">
   <si>
     <t>mouse</t>
   </si>
@@ -98,12 +99,18 @@
   </si>
   <si>
     <t>AWS</t>
+  </si>
+  <si>
+    <t>py_plot_ready</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,8 +212,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -302,6 +309,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -337,6 +361,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -512,11 +553,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,13 +565,14 @@
     <col min="1" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="8.88671875" style="4"/>
     <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="12.5546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="14.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,19 +592,22 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1322</v>
       </c>
@@ -579,16 +624,19 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1322</v>
       </c>
@@ -605,16 +653,19 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1322</v>
       </c>
@@ -631,16 +682,19 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1323</v>
       </c>
@@ -657,16 +711,19 @@
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1323</v>
       </c>
@@ -683,16 +740,19 @@
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1323</v>
       </c>
@@ -709,16 +769,19 @@
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1324</v>
       </c>
@@ -735,16 +798,19 @@
         <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1324</v>
       </c>
@@ -761,16 +827,19 @@
         <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1324</v>
       </c>
@@ -787,17 +856,17 @@
       <c r="F10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="1" t="b">
+      <c r="H10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1328</v>
       </c>
@@ -816,17 +885,17 @@
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1328</v>
       </c>
@@ -845,17 +914,17 @@
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1328</v>
       </c>
@@ -874,17 +943,17 @@
       <c r="F13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1328</v>
       </c>
@@ -903,17 +972,17 @@
       <c r="F14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1328</v>
       </c>
@@ -932,17 +1001,18 @@
       <c r="F15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="1" t="b">
+        <v>18</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1329</v>
       </c>
@@ -961,17 +1031,17 @@
       <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1329</v>
       </c>
@@ -987,14 +1057,14 @@
       <c r="E17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1329</v>
       </c>
@@ -1010,14 +1080,14 @@
       <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1329</v>
       </c>
@@ -1033,14 +1103,14 @@
       <c r="E19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1329</v>
       </c>
@@ -1056,14 +1126,14 @@
       <c r="E20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1337</v>
       </c>
@@ -1079,17 +1149,17 @@
       <c r="E21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1337</v>
       </c>
@@ -1105,14 +1175,14 @@
       <c r="E22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1337</v>
       </c>
@@ -1128,14 +1198,14 @@
       <c r="E23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1337</v>
       </c>
@@ -1151,14 +1221,14 @@
       <c r="E24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1337</v>
       </c>
@@ -1174,14 +1244,14 @@
       <c r="E25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1337</v>
       </c>
@@ -1197,14 +1267,14 @@
       <c r="E26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1338</v>
       </c>
@@ -1220,14 +1290,14 @@
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1338</v>
       </c>
@@ -1243,14 +1313,14 @@
       <c r="E28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1338</v>
       </c>
@@ -1266,14 +1336,14 @@
       <c r="E29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1338</v>
       </c>
@@ -1289,14 +1359,14 @@
       <c r="E30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1338</v>
       </c>
@@ -1312,14 +1382,14 @@
       <c r="E31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>1338</v>
       </c>
@@ -1338,14 +1408,14 @@
       <c r="F35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>1338</v>
       </c>
@@ -1364,14 +1434,14 @@
       <c r="F36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>1338</v>
       </c>
@@ -1387,17 +1457,17 @@
       <c r="E37" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>33303</v>
       </c>
@@ -1414,14 +1484,15 @@
         <v>12</v>
       </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="G38" s="5"/>
       <c r="H38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>33303</v>
       </c>
@@ -1437,14 +1508,14 @@
       <c r="E39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>33303</v>
       </c>
@@ -1460,14 +1531,14 @@
       <c r="E40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>33303</v>
       </c>
@@ -1483,14 +1554,14 @@
       <c r="E41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>33303</v>
       </c>
@@ -1506,14 +1577,14 @@
       <c r="E42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>33303</v>
       </c>
@@ -1532,14 +1603,14 @@
       <c r="F43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>33303</v>
       </c>
@@ -1555,14 +1626,14 @@
       <c r="E44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>33303</v>
       </c>
@@ -1581,17 +1652,17 @@
       <c r="F45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>33303</v>
       </c>
@@ -1607,14 +1678,14 @@
       <c r="E46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>33303</v>
       </c>
@@ -1633,14 +1704,14 @@
       <c r="F47" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>33303</v>
       </c>
@@ -1659,14 +1730,14 @@
       <c r="F48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>33303</v>
       </c>
@@ -1685,14 +1756,14 @@
       <c r="F49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>33303</v>
       </c>
@@ -1711,14 +1782,14 @@
       <c r="F50" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>33303</v>
       </c>
@@ -1734,10 +1805,10 @@
       <c r="E51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sbx to tif convert pipeline. before adjust caiman to pipeline
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10040009-FA77-46C2-A3D3-E2BF63286BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB09CF30-9330-443D-9F25-9B28ED7FF4CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1956" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="3160" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="31">
   <si>
     <t>mouse</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>caiman</t>
   </si>
 </sst>
 </file>
@@ -554,25 +557,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="8.88671875" style="4"/>
-    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="4" width="8.90625" style="1"/>
+    <col min="5" max="5" width="8.90625" style="4"/>
+    <col min="6" max="6" width="12.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" style="1"/>
+    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,10 +607,13 @@
         <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1322</v>
       </c>
@@ -635,8 +641,11 @@
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1322</v>
       </c>
@@ -661,11 +670,11 @@
       <c r="I3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="1" t="b">
+      <c r="L3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1322</v>
       </c>
@@ -690,11 +699,11 @@
       <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="1" t="b">
+      <c r="L4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1323</v>
       </c>
@@ -719,11 +728,14 @@
       <c r="I5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="1" t="b">
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1323</v>
       </c>
@@ -748,11 +760,11 @@
       <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="1" t="b">
+      <c r="L6" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1323</v>
       </c>
@@ -777,11 +789,11 @@
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="1" t="b">
+      <c r="L7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1324</v>
       </c>
@@ -809,8 +821,11 @@
       <c r="J8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1324</v>
       </c>
@@ -835,11 +850,11 @@
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="1" t="b">
+      <c r="L9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>1324</v>
       </c>
@@ -862,11 +877,11 @@
       <c r="I10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="1" t="b">
+      <c r="L10" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1328</v>
       </c>
@@ -891,11 +906,11 @@
       <c r="I11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="1" t="b">
+      <c r="L11" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1328</v>
       </c>
@@ -920,11 +935,11 @@
       <c r="I12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="1" t="b">
+      <c r="L12" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1328</v>
       </c>
@@ -949,11 +964,11 @@
       <c r="I13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="1" t="b">
+      <c r="L13" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1328</v>
       </c>
@@ -978,11 +993,11 @@
       <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="1" t="b">
+      <c r="L14" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1328</v>
       </c>
@@ -1008,11 +1023,11 @@
       <c r="I15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="1" t="b">
+      <c r="L15" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1329</v>
       </c>
@@ -1040,8 +1055,11 @@
       <c r="J16" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1329</v>
       </c>
@@ -1064,7 +1082,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1329</v>
       </c>
@@ -1087,7 +1105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1329</v>
       </c>
@@ -1110,7 +1128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1329</v>
       </c>
@@ -1133,7 +1151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1337</v>
       </c>
@@ -1158,8 +1176,11 @@
       <c r="J21" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1337</v>
       </c>
@@ -1181,8 +1202,11 @@
       <c r="I22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1337</v>
       </c>
@@ -1205,7 +1229,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1337</v>
       </c>
@@ -1228,7 +1252,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1337</v>
       </c>
@@ -1251,7 +1275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1337</v>
       </c>
@@ -1274,7 +1298,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1338</v>
       </c>
@@ -1296,8 +1320,11 @@
       <c r="I27" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1338</v>
       </c>
@@ -1319,8 +1346,11 @@
       <c r="I28" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1338</v>
       </c>
@@ -1343,7 +1373,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1338</v>
       </c>
@@ -1366,7 +1396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>1338</v>
       </c>
@@ -1389,7 +1419,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>1338</v>
       </c>
@@ -1415,7 +1445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>1338</v>
       </c>
@@ -1441,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>1338</v>
       </c>
@@ -1467,7 +1497,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>33303</v>
       </c>
@@ -1492,7 +1522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>33303</v>
       </c>
@@ -1515,7 +1545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>33303</v>
       </c>
@@ -1538,7 +1568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>33303</v>
       </c>
@@ -1561,7 +1591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>33303</v>
       </c>
@@ -1584,7 +1614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>33303</v>
       </c>
@@ -1610,7 +1640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>33303</v>
       </c>
@@ -1633,7 +1663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>33303</v>
       </c>
@@ -1662,7 +1692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>33303</v>
       </c>
@@ -1685,7 +1715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>33303</v>
       </c>
@@ -1711,7 +1741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>33303</v>
       </c>
@@ -1737,7 +1767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>33303</v>
       </c>
@@ -1763,7 +1793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>33303</v>
       </c>
@@ -1789,7 +1819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>33303</v>
       </c>

</xml_diff>

<commit_message>
fix recording num bug in master xls
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB09CF30-9330-443D-9F25-9B28ED7FF4CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF2848-DFBC-4792-89D3-E2F09622D44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3160" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="3760" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="31">
   <si>
     <t>mouse</t>
   </si>
@@ -560,7 +560,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,6 +626,9 @@
       <c r="D2" s="1">
         <v>200</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
@@ -716,6 +719,9 @@
       <c r="D5" s="1">
         <v>200</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
@@ -805,6 +811,9 @@
       </c>
       <c r="D8" s="1">
         <v>200</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
tidy up sbx to tiff & modify for bunny500
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF2848-DFBC-4792-89D3-E2F09622D44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FC209D-BDC9-457B-9697-AAF8EF53655B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3760" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="4360" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="32">
   <si>
     <t>mouse</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>caiman</t>
+  </si>
+  <si>
+    <t>bunny500</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1428,138 +1431,162 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B33" s="1">
+        <v>210922</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>200</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B34" s="1">
+        <v>210922</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>200</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B35" s="1">
+        <v>210922</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>200</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="37" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5">
         <v>1338</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B37" s="5">
         <v>210602</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="5">
-        <v>200</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="5" t="s">
+      <c r="C37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5">
+        <v>200</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5">
+      <c r="I37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
         <v>1338</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B38" s="5">
         <v>210609</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="5">
-        <v>200</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="5" t="s">
+      <c r="C38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="5">
+        <v>200</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+      <c r="I38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
         <v>1338</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B39" s="2">
         <v>210616</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2">
-        <v>200</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>200</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J37" s="2" t="s">
+      <c r="I39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B38" s="1">
-        <v>210401</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1">
-        <v>150</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B39" s="1">
-        <v>210405</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1">
-        <v>150</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>33303</v>
       </c>
       <c r="B40" s="1">
-        <v>210415</v>
+        <v>210401</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
@@ -1568,8 +1595,10 @@
         <v>150</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
       <c r="H40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1577,21 +1606,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>33303</v>
       </c>
       <c r="B41" s="1">
-        <v>210415</v>
+        <v>210405</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>18</v>
@@ -1600,18 +1629,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>33303</v>
       </c>
       <c r="B42" s="1">
-        <v>210419</v>
+        <v>210415</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>11</v>
@@ -1623,24 +1652,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>33303</v>
       </c>
-      <c r="B43" s="8">
-        <v>210419</v>
+      <c r="B43" s="1">
+        <v>210415</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="8">
-        <v>150</v>
+      <c r="D43" s="1">
+        <v>200</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>18</v>
@@ -1649,12 +1675,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>33303</v>
       </c>
       <c r="B44" s="1">
-        <v>210422</v>
+        <v>210419</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
@@ -1672,12 +1698,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>33303</v>
       </c>
       <c r="B45" s="8">
-        <v>210422</v>
+        <v>210419</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
@@ -1686,7 +1712,7 @@
         <v>150</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>24</v>
@@ -1697,16 +1723,13 @@
       <c r="I45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>33303</v>
       </c>
-      <c r="B46" s="2">
-        <v>210430</v>
+      <c r="B46" s="1">
+        <v>210422</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
@@ -1724,21 +1747,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>33303</v>
       </c>
-      <c r="B47" s="3">
-        <v>210430</v>
+      <c r="B47" s="8">
+        <v>210422</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="8">
         <v>150</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>24</v>
@@ -1749,25 +1772,25 @@
       <c r="I47" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>33303</v>
       </c>
-      <c r="B48" s="3">
-        <v>210506</v>
+      <c r="B48" s="2">
+        <v>210430</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="1">
         <v>200</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>18</v>
@@ -1780,17 +1803,17 @@
       <c r="A49" s="1">
         <v>33303</v>
       </c>
-      <c r="B49" s="8">
-        <v>210603</v>
+      <c r="B49" s="3">
+        <v>210430</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D49" s="3">
         <v>150</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>24</v>
@@ -1806,14 +1829,14 @@
       <c r="A50" s="1">
         <v>33303</v>
       </c>
-      <c r="B50" s="8">
-        <v>210610</v>
+      <c r="B50" s="3">
+        <v>210506</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="8">
-        <v>150</v>
+      <c r="D50" s="3">
+        <v>200</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>11</v>
@@ -1832,22 +1855,74 @@
       <c r="A51" s="1">
         <v>33303</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="8">
+        <v>210603</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="8">
+        <v>150</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B52" s="8">
+        <v>210610</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="8">
+        <v>150</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B53" s="1">
         <v>210617</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="1">
+      <c r="C53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1">
         <v>150</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I51" s="1" t="s">
+      <c r="E53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran caiman on LM bunnytop, running on high resolution bunnytop
</commit_message>
<xml_diff>
--- a/mat/adp_dataset_master.xlsx
+++ b/mat/adp_dataset_master.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B5231-048F-4800-B2BD-1009FDC936F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F649FB39-2149-40B1-9548-A5785097A25F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="5560" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="6160" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="34">
   <si>
     <t>mouse</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>bunnytop</t>
+  </si>
+  <si>
+    <t>bunnytop high res</t>
   </si>
 </sst>
 </file>
@@ -563,22 +566,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.90625" style="1"/>
-    <col min="5" max="5" width="8.90625" style="4"/>
-    <col min="6" max="6" width="12.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.90625" style="1"/>
-    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1704,100 +1712,81 @@
       </c>
     </row>
     <row r="46" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E46" s="7"/>
-      <c r="I46" s="1"/>
+      <c r="A46" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B46" s="2">
+        <v>220225</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>200</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="47" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E47" s="7"/>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B48" s="1">
-        <v>210401</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="1">
-        <v>150</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="A47" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B47" s="2">
+        <v>220225</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2">
+        <v>200</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B49" s="1">
-        <v>210405</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="1">
-        <v>150</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B50" s="1">
-        <v>210415</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="1">
-        <v>150</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="H47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E48" s="7"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E49" s="7"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E50" s="7"/>
+      <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>33303</v>
       </c>
       <c r="B51" s="1">
-        <v>210415</v>
+        <v>210401</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
       <c r="H51" s="1" t="s">
         <v>18</v>
       </c>
@@ -1810,16 +1799,16 @@
         <v>33303</v>
       </c>
       <c r="B52" s="1">
-        <v>210419</v>
+        <v>210405</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D52" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>18</v>
@@ -1832,20 +1821,17 @@
       <c r="A53" s="1">
         <v>33303</v>
       </c>
-      <c r="B53" s="8">
-        <v>210419</v>
+      <c r="B53" s="1">
+        <v>210415</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="1">
         <v>150</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>18</v>
@@ -1859,7 +1845,7 @@
         <v>33303</v>
       </c>
       <c r="B54" s="1">
-        <v>210422</v>
+        <v>210415</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>3</v>
@@ -1868,7 +1854,7 @@
         <v>200</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>18</v>
@@ -1881,46 +1867,43 @@
       <c r="A55" s="1">
         <v>33303</v>
       </c>
-      <c r="B55" s="8">
-        <v>210422</v>
+      <c r="B55" s="1">
+        <v>210419</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="8">
-        <v>150</v>
+      <c r="D55" s="1">
+        <v>200</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>33303</v>
       </c>
-      <c r="B56" s="2">
-        <v>210430</v>
+      <c r="B56" s="8">
+        <v>210419</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="1">
-        <v>200</v>
+      <c r="D56" s="8">
+        <v>150</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>18</v>
@@ -1933,20 +1916,17 @@
       <c r="A57" s="1">
         <v>33303</v>
       </c>
-      <c r="B57" s="3">
-        <v>210430</v>
+      <c r="B57" s="1">
+        <v>210422</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="3">
-        <v>150</v>
+      <c r="D57" s="1">
+        <v>200</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>18</v>
@@ -1959,17 +1939,17 @@
       <c r="A58" s="1">
         <v>33303</v>
       </c>
-      <c r="B58" s="3">
-        <v>210506</v>
+      <c r="B58" s="8">
+        <v>210422</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="3">
-        <v>200</v>
+      <c r="D58" s="8">
+        <v>150</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>24</v>
@@ -1979,26 +1959,26 @@
       </c>
       <c r="I58" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>33303</v>
       </c>
-      <c r="B59" s="8">
-        <v>210603</v>
+      <c r="B59" s="2">
+        <v>210430</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D59" s="8">
-        <v>150</v>
+      <c r="D59" s="1">
+        <v>200</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>18</v>
@@ -2011,17 +1991,17 @@
       <c r="A60" s="1">
         <v>33303</v>
       </c>
-      <c r="B60" s="8">
-        <v>210610</v>
+      <c r="B60" s="3">
+        <v>210430</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="3">
         <v>150</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>24</v>
@@ -2037,22 +2017,100 @@
       <c r="A61" s="1">
         <v>33303</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="3">
+        <v>210506</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="3">
+        <v>200</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B62" s="8">
+        <v>210603</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="8">
+        <v>150</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B63" s="8">
+        <v>210610</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="8">
+        <v>150</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B64" s="1">
         <v>210617</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="1">
+      <c r="C64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1">
         <v>150</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I61" s="1" t="s">
+      <c r="E64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>